<commit_message>
format: output 2 endline for each top config message
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34591D7B-9892-4077-917D-C66D9AD77636}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30AE39E-60D4-43B6-90E0-79C76C430198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10485" yWindow="10215" windowWidth="44280" windowHeight="13800" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-2040" yWindow="6420" windowWidth="44280" windowHeight="13815" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
+    <sheet name="Reward" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -244,6 +245,45 @@
   </si>
   <si>
     <t>目标</t>
+  </si>
+  <si>
+    <t>map&lt;uint32, Reward&gt;</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>奖励ID</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>奖励1</t>
+  </si>
+  <si>
+    <t>奖励2</t>
+  </si>
+  <si>
+    <t>Item1Id</t>
+  </si>
+  <si>
+    <t>Item1Num</t>
+  </si>
+  <si>
+    <t>Item2Id</t>
+  </si>
+  <si>
+    <t>Item2Num</t>
+  </si>
+  <si>
+    <t>Item3Id</t>
+  </si>
+  <si>
+    <t>Item3Num</t>
   </si>
 </sst>
 </file>
@@ -285,7 +325,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -308,11 +348,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -333,6 +382,12 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -649,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U9" sqref="U9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1189,4 +1244,153 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD500D4-49FD-425F-87E7-4971CEE20F74}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2002</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>2002</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5">
+        <v>2001</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2007</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: support horizontal scalar list
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30AE39E-60D4-43B6-90E0-79C76C430198}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7B7C6E-C12C-424C-AC33-4BDBDE8945A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2040" yWindow="6420" windowWidth="44280" windowHeight="13815" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="7530" yWindow="7260" windowWidth="44280" windowHeight="13440" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -284,6 +284,27 @@
   </si>
   <si>
     <t>Item3Num</t>
+  </si>
+  <si>
+    <t>ClientParam1</t>
+  </si>
+  <si>
+    <t>ClientParam2</t>
+  </si>
+  <si>
+    <t>ClientParam3</t>
+  </si>
+  <si>
+    <t>客户端参数1</t>
+  </si>
+  <si>
+    <t>客户端参数2</t>
+  </si>
+  <si>
+    <t>客户端参数3</t>
+  </si>
+  <si>
+    <t>[]string</t>
   </si>
 </sst>
 </file>
@@ -702,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:L4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -725,9 +746,12 @@
     <col min="13" max="13" width="20.125" customWidth="1"/>
     <col min="14" max="14" width="19.375" customWidth="1"/>
     <col min="15" max="15" width="15.5" style="1" customWidth="1"/>
+    <col min="21" max="21" width="13.75" customWidth="1"/>
+    <col min="22" max="22" width="14.625" customWidth="1"/>
+    <col min="23" max="23" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -788,8 +812,17 @@
       <c r="T1" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="U1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -850,8 +883,17 @@
       <c r="T2" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="U2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -909,8 +951,17 @@
       <c r="T3" s="6" t="s">
         <v>70</v>
       </c>
+      <c r="U3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -953,16 +1004,25 @@
         <v>17</v>
       </c>
       <c r="P4" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q4" s="1">
         <v>1</v>
       </c>
       <c r="T4" s="1">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+      <c r="W4" s="1">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1013,8 +1073,14 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
+      <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1058,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1081,7 +1147,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1134,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100002</v>
       </c>
@@ -1187,7 +1253,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100003</v>
       </c>
@@ -1251,7 +1317,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: nested message type merge
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7B7C6E-C12C-424C-AC33-4BDBDE8945A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E26CB0-A81F-40EA-A88C-12C02DA6F618}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7530" yWindow="7260" windowWidth="44280" windowHeight="13440" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="3540" yWindow="7365" windowWidth="35040" windowHeight="13425" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -268,24 +268,6 @@
     <t>奖励2</t>
   </si>
   <si>
-    <t>Item1Id</t>
-  </si>
-  <si>
-    <t>Item1Num</t>
-  </si>
-  <si>
-    <t>Item2Id</t>
-  </si>
-  <si>
-    <t>Item2Num</t>
-  </si>
-  <si>
-    <t>Item3Id</t>
-  </si>
-  <si>
-    <t>Item3Num</t>
-  </si>
-  <si>
     <t>ClientParam1</t>
   </si>
   <si>
@@ -305,6 +287,78 @@
   </si>
   <si>
     <t>[]string</t>
+  </si>
+  <si>
+    <t>InputItem1Id</t>
+  </si>
+  <si>
+    <t>InputItem1Num</t>
+  </si>
+  <si>
+    <t>InputItem2Id</t>
+  </si>
+  <si>
+    <t>InputItem2Num</t>
+  </si>
+  <si>
+    <t>InputItem3Id</t>
+  </si>
+  <si>
+    <t>InputItem3Num</t>
+  </si>
+  <si>
+    <t>OutputItem1Id</t>
+  </si>
+  <si>
+    <t>OutputItem1Num</t>
+  </si>
+  <si>
+    <t>OutputItem2Id</t>
+  </si>
+  <si>
+    <t>OutputItem2Num</t>
+  </si>
+  <si>
+    <t>[Exchange]uint32</t>
+  </si>
+  <si>
+    <t>ExchangeId</t>
+  </si>
+  <si>
+    <t>奖励3</t>
+  </si>
+  <si>
+    <t>兑换ID</t>
+  </si>
+  <si>
+    <t>RewardItem1Num</t>
+  </si>
+  <si>
+    <t>RewardItem1Id</t>
+  </si>
+  <si>
+    <t>RewardItem2Id</t>
+  </si>
+  <si>
+    <t>RewardItem2Num</t>
+  </si>
+  <si>
+    <t>道具1Id</t>
+  </si>
+  <si>
+    <t>道具1Num</t>
+  </si>
+  <si>
+    <t>道具2Id</t>
+  </si>
+  <si>
+    <t>道具2Num</t>
+  </si>
+  <si>
+    <t>道具3Id</t>
+  </si>
+  <si>
+    <t>道具3Num</t>
   </si>
 </sst>
 </file>
@@ -813,13 +867,13 @@
         <v>68</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -884,7 +938,7 @@
         <v>57</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>34</v>
@@ -952,13 +1006,13 @@
         <v>70</v>
       </c>
       <c r="U3" s="6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="W3" s="6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1314,25 +1368,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD500D4-49FD-425F-87E7-4971CEE20F74}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
@@ -1340,25 +1403,52 @@
         <v>74</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>71</v>
       </c>
@@ -1378,13 +1468,40 @@
         <v>57</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
@@ -1403,14 +1520,41 @@
       <c r="F3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>31</v>
+      <c r="G3" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>28</v>
+        <v>103</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1418,41 +1562,165 @@
         <v>76</v>
       </c>
       <c r="C4">
-        <v>2002</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>2002</v>
       </c>
       <c r="E4">
-        <v>2002</v>
+        <v>2</v>
       </c>
       <c r="F4">
+        <v>2002</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2002</v>
+      </c>
+      <c r="I4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>2002</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
+        <v>2002</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>2002</v>
+      </c>
+      <c r="M4">
         <v>3</v>
       </c>
+      <c r="N4">
+        <v>2002</v>
+      </c>
+      <c r="O4">
+        <v>3</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
       </c>
       <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2002</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>2002</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2002</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>2002</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>2002</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5">
+        <v>2002</v>
+      </c>
+      <c r="O5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2002</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2002</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>2002</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2002</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>2002</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>2001</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="G5">
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
         <v>2007</v>
       </c>
-      <c r="H5">
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7">
+        <v>2001</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>2007</v>
+      </c>
+      <c r="O7">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: imports injection, same message type merge
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Development/GitHub/tableau/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E26CB0-A81F-40EA-A88C-12C02DA6F618}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2906C28-98FA-0845-9CC1-EA1B780B30F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="7365" windowWidth="35040" windowHeight="13425" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1840" yWindow="2620" windowWidth="30720" windowHeight="13420" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="112">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -359,6 +359,15 @@
   </si>
   <si>
     <t>道具3Num</t>
+  </si>
+  <si>
+    <t>奖励4</t>
+  </si>
+  <si>
+    <t>[.Item]int32</t>
+  </si>
+  <si>
+    <t>[OutputItem]int32</t>
   </si>
 </sst>
 </file>
@@ -465,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -481,7 +490,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -783,29 +792,29 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="18.75" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
-    <col min="6" max="6" width="19.375" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
-    <col min="12" max="12" width="16.75" customWidth="1"/>
-    <col min="13" max="13" width="20.125" customWidth="1"/>
-    <col min="14" max="14" width="19.375" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="20.1640625" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1"/>
     <col min="15" max="15" width="15.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.75" customWidth="1"/>
-    <col min="22" max="22" width="14.625" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
     <col min="23" max="23" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -876,7 +885,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -947,7 +956,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1015,7 +1024,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1076,7 +1085,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1201,7 +1210,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1254,7 +1263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>100002</v>
       </c>
@@ -1307,7 +1316,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>100003</v>
       </c>
@@ -1371,31 +1380,31 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
@@ -1448,7 +1457,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>71</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>57</v>
@@ -1471,7 +1480,7 @@
         <v>95</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>57</v>
@@ -1489,7 +1498,7 @@
         <v>57</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>57</v>
@@ -1501,7 +1510,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
@@ -1554,7 +1563,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1601,9 +1610,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>77</v>
@@ -1648,9 +1657,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>97</v>
@@ -1689,12 +1698,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C7">
         <v>1</v>

</xml_diff>

<commit_message>
feat: incell list, map, and struct
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wenchyzhu/Development/GitHub/tableau/test/testdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2906C28-98FA-0845-9CC1-EA1B780B30F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C017E92-CE1F-44B7-9E7F-17BBFF4660F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="2620" windowWidth="30720" windowHeight="13420" activeTab="1" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-18060" yWindow="9615" windowWidth="43335" windowHeight="13425" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -367,7 +367,46 @@
     <t>[.Item]int32</t>
   </si>
   <si>
-    <t>[OutputItem]int32</t>
+    <t>[ExchangeItem]int32</t>
+  </si>
+  <si>
+    <t>IntParams</t>
+  </si>
+  <si>
+    <t>[]int32</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>整型参数列表</t>
+  </si>
+  <si>
+    <t>Tips</t>
+  </si>
+  <si>
+    <t>1:good,2:bad</t>
+  </si>
+  <si>
+    <t>10:hot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map&lt;int32,string&gt; </t>
+  </si>
+  <si>
+    <t>WarnInfo</t>
+  </si>
+  <si>
+    <t>1,desc1,100</t>
+  </si>
+  <si>
+    <t>2,desc2,500</t>
+  </si>
+  <si>
+    <t>3,desc3,1000</t>
+  </si>
+  <si>
+    <t>{int32 Id,string Desc,int32 Value}Info</t>
   </si>
 </sst>
 </file>
@@ -474,7 +513,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,7 +529,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -786,35 +825,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="19.375" customWidth="1"/>
     <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.875" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="15.1640625" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="20.1640625" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.625" customWidth="1"/>
+    <col min="11" max="11" width="15.125" customWidth="1"/>
+    <col min="12" max="12" width="16.625" customWidth="1"/>
+    <col min="13" max="13" width="20.125" customWidth="1"/>
+    <col min="14" max="14" width="19.375" customWidth="1"/>
     <col min="15" max="15" width="15.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.6640625" customWidth="1"/>
-    <col min="23" max="23" width="14.5" customWidth="1"/>
+    <col min="21" max="21" width="32" customWidth="1"/>
+    <col min="22" max="22" width="13.625" customWidth="1"/>
+    <col min="23" max="23" width="16.25" customWidth="1"/>
+    <col min="24" max="26" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -876,16 +916,25 @@
         <v>68</v>
       </c>
       <c r="U1" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -947,16 +996,25 @@
         <v>57</v>
       </c>
       <c r="U2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="X2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="Y2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="Z2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1014,17 +1072,23 @@
       <c r="T3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="W3" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="X3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="Z3" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1075,17 +1139,14 @@
       <c r="T4" s="1">
         <v>10</v>
       </c>
-      <c r="U4" s="1">
-        <v>1</v>
+      <c r="U4" s="1" t="s">
+        <v>121</v>
       </c>
       <c r="V4" s="1">
-        <v>2</v>
-      </c>
-      <c r="W4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1136,14 +1197,17 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
-      <c r="U5" s="1">
-        <v>4</v>
+      <c r="U5" s="1" t="s">
+        <v>122</v>
       </c>
       <c r="V5" s="1">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1186,8 +1250,17 @@
       <c r="T6" s="1">
         <v>1</v>
       </c>
+      <c r="U6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1210,7 +1283,7 @@
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1263,7 +1336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100002</v>
       </c>
@@ -1316,7 +1389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100003</v>
       </c>
@@ -1379,32 +1452,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD500D4-49FD-425F-87E7-4971CEE20F74}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" customWidth="1"/>
-    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.375" customWidth="1"/>
+    <col min="15" max="15" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>72</v>
       </c>
@@ -1457,7 +1530,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>71</v>
       </c>
@@ -1480,7 +1553,7 @@
         <v>95</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I2" s="4" t="s">
         <v>57</v>
@@ -1510,7 +1583,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>73</v>
       </c>
@@ -1563,7 +1636,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1610,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1657,7 +1730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1698,7 +1771,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
feat: infinite nested types
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C017E92-CE1F-44B7-9E7F-17BBFF4660F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CA055-9266-40CC-9924-3C32F5E643A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18060" yWindow="9615" windowWidth="43335" windowHeight="13425" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-19530" yWindow="9090" windowWidth="42480" windowHeight="13980" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="135">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -181,15 +181,6 @@
     <t>SectionItem3Num</t>
   </si>
   <si>
-    <t>BeginTime</t>
-  </si>
-  <si>
-    <t>Duration</t>
-  </si>
-  <si>
-    <t>EndTime</t>
-  </si>
-  <si>
     <t>timestamp</t>
   </si>
   <si>
@@ -407,6 +398,45 @@
   </si>
   <si>
     <t>{int32 Id,string Desc,int32 Value}Info</t>
+  </si>
+  <si>
+    <t>DurationType</t>
+  </si>
+  <si>
+    <t>{Duration}int32</t>
+  </si>
+  <si>
+    <t>DurationBeginTime</t>
+  </si>
+  <si>
+    <t>DurationEndTime</t>
+  </si>
+  <si>
+    <t>Timespan</t>
+  </si>
+  <si>
+    <t>DurationParams</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>IncellStruct</t>
+  </si>
+  <si>
+    <t>1,desc</t>
+  </si>
+  <si>
+    <t>1,desc2</t>
+  </si>
+  <si>
+    <t>1,desc3</t>
+  </si>
+  <si>
+    <t>{int32 Id,string Desc}Info</t>
   </si>
 </sst>
 </file>
@@ -825,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -844,17 +874,18 @@
     <col min="9" max="9" width="15" customWidth="1"/>
     <col min="10" max="10" width="15.625" customWidth="1"/>
     <col min="11" max="11" width="15.125" customWidth="1"/>
-    <col min="12" max="12" width="16.625" customWidth="1"/>
-    <col min="13" max="13" width="20.125" customWidth="1"/>
-    <col min="14" max="14" width="19.375" customWidth="1"/>
-    <col min="15" max="15" width="15.5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="32" customWidth="1"/>
-    <col min="22" max="22" width="13.625" customWidth="1"/>
-    <col min="23" max="23" width="16.25" customWidth="1"/>
-    <col min="24" max="26" width="12.375" customWidth="1"/>
+    <col min="12" max="13" width="16.625" customWidth="1"/>
+    <col min="14" max="14" width="20.125" customWidth="1"/>
+    <col min="15" max="16" width="19.375" customWidth="1"/>
+    <col min="17" max="17" width="18.625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="32" customWidth="1"/>
+    <col min="24" max="24" width="23.375" customWidth="1"/>
+    <col min="25" max="25" width="13.625" customWidth="1"/>
+    <col min="26" max="26" width="16.25" customWidth="1"/>
+    <col min="27" max="29" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -892,51 +923,60 @@
         <v>48</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>50</v>
+        <v>124</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="W1" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>80</v>
+        <v>113</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -954,67 +994,76 @@
         <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>52</v>
+        <v>123</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>57</v>
+        <v>110</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>50</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>124</v>
+        <v>54</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>113</v>
+        <v>54</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="Y2" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1048,52 +1097,56 @@
       <c r="L3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="P3" s="7"/>
+      <c r="Q3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="R3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Q3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>70</v>
-      </c>
       <c r="V3" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="X3" s="6" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1121,37 +1174,46 @@
       <c r="L4" s="2">
         <v>10</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>9</v>
       </c>
-      <c r="Q4" s="1">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1">
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="V4" s="1">
         <v>10</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="V4" s="1">
+      <c r="W4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1179,40 +1241,49 @@
       <c r="L5" s="2">
         <v>5</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M5" s="2">
+        <v>2</v>
+      </c>
+      <c r="N5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="O5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="P5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>2</v>
-      </c>
-      <c r="T5" s="1">
-        <v>1</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>122</v>
+      <c r="R5" s="1">
+        <v>1</v>
+      </c>
+      <c r="S5" s="1">
+        <v>2</v>
       </c>
       <c r="V5" s="1">
         <v>1</v>
       </c>
       <c r="W5" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1232,40 +1303,49 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="3" t="s">
+      <c r="M6" s="2">
+        <v>3</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="P6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="P6" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="1">
+      <c r="R6" s="1">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1">
         <v>3</v>
       </c>
-      <c r="T6" s="1">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="1">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z6" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>117</v>
-      </c>
     </row>
-    <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1279,16 +1359,18 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="3"/>
+      <c r="M7" s="2"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
-    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1320,28 +1402,32 @@
       <c r="L8" s="2">
         <v>3</v>
       </c>
-      <c r="M8" s="3" t="s">
+      <c r="M8" s="2">
+        <v>2</v>
+      </c>
+      <c r="N8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="3" t="s">
+      <c r="O8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="P8" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="1">
+      <c r="R8" s="1">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100002</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1373,28 +1459,32 @@
       <c r="L9" s="2">
         <v>2</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="P9" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="R9" s="1">
+        <v>2</v>
+      </c>
+      <c r="S9" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100003</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1426,19 +1516,23 @@
       <c r="L10" s="2">
         <v>2</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="M10" s="2">
+        <v>2</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="P10" s="1">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="R10" s="1">
+        <v>2</v>
+      </c>
+      <c r="S10" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1479,116 +1573,116 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>29</v>
@@ -1603,25 +1697,25 @@
         <v>27</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>105</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>108</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>29</v>
@@ -1641,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1688,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1735,7 +1829,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -1776,7 +1870,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C7">
         <v>1</v>

</xml_diff>

<commit_message>
fix: protogen parser: struct cursor
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CA055-9266-40CC-9924-3C32F5E643A6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDAA3CB-602B-4BD3-B334-FA0D254FD3E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19530" yWindow="9090" windowWidth="42480" windowHeight="13980" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-6840" yWindow="5565" windowWidth="34965" windowHeight="14730" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="134">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -434,9 +434,6 @@
   </si>
   <si>
     <t>1,desc3</t>
-  </si>
-  <si>
-    <t>{int32 Id,string Desc}Info</t>
   </si>
 </sst>
 </file>
@@ -857,8 +854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="X10" sqref="X10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X8" sqref="X8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -879,7 +876,7 @@
     <col min="15" max="16" width="19.375" customWidth="1"/>
     <col min="17" max="17" width="18.625" style="1" customWidth="1"/>
     <col min="23" max="23" width="32" customWidth="1"/>
-    <col min="24" max="24" width="23.375" customWidth="1"/>
+    <col min="24" max="24" width="30.75" customWidth="1"/>
     <col min="25" max="25" width="13.625" customWidth="1"/>
     <col min="26" max="26" width="16.25" customWidth="1"/>
     <col min="27" max="29" width="12.375" customWidth="1"/>
@@ -1045,7 +1042,7 @@
         <v>121</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>110</v>

</xml_diff>

<commit_message>
feat: support enum type, fix imports
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADDAA3CB-602B-4BD3-B334-FA0D254FD3E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372DA76C-6AC2-42C9-B971-BB2D2F8F1224}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6840" yWindow="5565" windowWidth="34965" windowHeight="14730" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-510" yWindow="8895" windowWidth="38670" windowHeight="15105" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="139">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -403,15 +403,6 @@
     <t>DurationType</t>
   </si>
   <si>
-    <t>{Duration}int32</t>
-  </si>
-  <si>
-    <t>DurationBeginTime</t>
-  </si>
-  <si>
-    <t>DurationEndTime</t>
-  </si>
-  <si>
     <t>Timespan</t>
   </si>
   <si>
@@ -434,6 +425,30 @@
   </si>
   <si>
     <t>1,desc3</t>
+  </si>
+  <si>
+    <t>开服时间</t>
+  </si>
+  <si>
+    <t>DURATION_TYPE_REGISTER</t>
+  </si>
+  <si>
+    <t>DurationBegin</t>
+  </si>
+  <si>
+    <t>DurationEnd</t>
+  </si>
+  <si>
+    <t>延迟天数</t>
+  </si>
+  <si>
+    <t>自定义参数</t>
+  </si>
+  <si>
+    <t>{.Duration}enum&lt;.DurationType&gt;</t>
+  </si>
+  <si>
+    <t>DurationDelayedDays</t>
   </si>
 </sst>
 </file>
@@ -852,37 +867,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="14.125" customWidth="1"/>
-    <col min="6" max="6" width="19.375" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
-    <col min="8" max="8" width="16.875" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="15.625" customWidth="1"/>
-    <col min="11" max="11" width="15.125" customWidth="1"/>
-    <col min="12" max="13" width="16.625" customWidth="1"/>
-    <col min="14" max="14" width="20.125" customWidth="1"/>
-    <col min="15" max="16" width="19.375" customWidth="1"/>
-    <col min="17" max="17" width="18.625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="32" customWidth="1"/>
-    <col min="24" max="24" width="30.75" customWidth="1"/>
-    <col min="25" max="25" width="13.625" customWidth="1"/>
-    <col min="26" max="26" width="16.25" customWidth="1"/>
-    <col min="27" max="29" width="12.375" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.625" customWidth="1"/>
+    <col min="14" max="15" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.625" customWidth="1"/>
+    <col min="17" max="17" width="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.25" customWidth="1"/>
+    <col min="28" max="30" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>32</v>
       </c>
@@ -923,55 +942,58 @@
         <v>122</v>
       </c>
       <c r="N1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Q1" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
@@ -1009,7 +1031,7 @@
         <v>54</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>49</v>
@@ -1018,16 +1040,16 @@
         <v>49</v>
       </c>
       <c r="P2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>54</v>
@@ -1039,28 +1061,31 @@
         <v>54</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>121</v>
+        <v>54</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>121</v>
       </c>
       <c r="Y2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z2" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>34</v>
       </c>
       <c r="AC2" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="AD2" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1100,45 +1125,50 @@
       <c r="O3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="6" t="s">
+      <c r="P3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="Y3" s="6" t="s">
         <v>112</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="AA3" s="6" t="s">
         <v>78</v>
       </c>
       <c r="AB3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC3" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1171,41 +1201,42 @@
       <c r="L4" s="2">
         <v>10</v>
       </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
+      <c r="M4" s="2"/>
       <c r="N4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="P4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="1">
+        <v>9</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+      <c r="W4" s="1">
+        <v>10</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="1">
-        <v>9</v>
-      </c>
-      <c r="S4" s="1">
-        <v>1</v>
-      </c>
-      <c r="V4" s="1">
-        <v>10</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y4" s="1">
+      <c r="Z4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1222,60 +1253,60 @@
         <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2">
-        <v>2003</v>
-      </c>
-      <c r="J5" s="2">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2001</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
       <c r="K5" s="2">
         <v>2007</v>
       </c>
       <c r="L5" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" s="3" t="s">
-        <v>129</v>
+      <c r="P5" s="1">
+        <v>1</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R5" s="1">
-        <v>1</v>
+        <v>125</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="S5" s="1">
-        <v>2</v>
-      </c>
-      <c r="V5" s="1">
-        <v>1</v>
-      </c>
-      <c r="W5" s="1" t="s">
-        <v>119</v>
+        <v>9</v>
+      </c>
+      <c r="T5" s="1">
+        <v>1</v>
+      </c>
+      <c r="W5" s="1">
+        <v>10</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>115</v>
+        <v>118</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1292,16 +1323,24 @@
         <v>3</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>3</v>
+      <c r="I6" s="2">
+        <v>2003</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2007</v>
+      </c>
+      <c r="L6" s="2">
+        <v>5</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>21</v>
@@ -1309,35 +1348,38 @@
       <c r="O6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="3" t="s">
-        <v>111</v>
+      <c r="P6" s="1">
+        <v>2</v>
       </c>
       <c r="Q6" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R6" s="1">
-        <v>1</v>
-      </c>
       <c r="S6" s="1">
-        <v>3</v>
-      </c>
-      <c r="V6" s="1">
-        <v>1</v>
-      </c>
-      <c r="W6" s="1" t="s">
-        <v>120</v>
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>2</v>
+      </c>
+      <c r="W6" s="1">
+        <v>1</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>114</v>
+        <v>129</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1349,6 +1391,12 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1356,13 +1404,47 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="M7" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1">
+        <v>3</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1370,130 +1452,101 @@
         <v>51</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>100001</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1" t="s">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="2">
-        <v>2002</v>
-      </c>
-      <c r="H8" s="2">
-        <v>2</v>
-      </c>
-      <c r="I8" s="2">
-        <v>2002</v>
-      </c>
-      <c r="J8" s="2">
+      <c r="G9" s="2">
+        <v>2002</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>2002</v>
+      </c>
+      <c r="J9" s="2">
         <v>3</v>
       </c>
-      <c r="K8" s="2">
-        <v>2002</v>
-      </c>
-      <c r="L8" s="2">
+      <c r="K9" s="2">
+        <v>2002</v>
+      </c>
+      <c r="L9" s="2">
         <v>3</v>
       </c>
-      <c r="M8" s="2">
-        <v>2</v>
-      </c>
-      <c r="N8" s="3" t="s">
+      <c r="M9" s="2">
+        <v>2</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3" t="s">
+      <c r="P9" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R8" s="1">
-        <v>2</v>
-      </c>
-      <c r="S8" s="1">
+      <c r="S9" s="1">
+        <v>2</v>
+      </c>
+      <c r="T9" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>100002</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E10" s="1">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2001</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2">
-        <v>2002</v>
-      </c>
-      <c r="J9" s="2">
-        <v>2</v>
-      </c>
-      <c r="K9" s="2">
-        <v>2002</v>
-      </c>
-      <c r="L9" s="2">
-        <v>2</v>
-      </c>
-      <c r="M9" s="2">
-        <v>2</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" s="1">
-        <v>2</v>
-      </c>
-      <c r="S9" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>100003</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="G10" s="2">
         <v>2001</v>
@@ -1517,19 +1570,82 @@
         <v>2</v>
       </c>
       <c r="N10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="P10" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="1">
+        <v>2</v>
+      </c>
+      <c r="T10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>100003</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>2001</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2">
+        <v>2002</v>
+      </c>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2002</v>
+      </c>
+      <c r="L11" s="2">
+        <v>2</v>
+      </c>
+      <c r="M11" s="2">
+        <v>2</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3" t="s">
+      <c r="P11" s="1">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="R10" s="1">
-        <v>2</v>
-      </c>
-      <c r="S10" s="1">
+      <c r="S11" s="1">
+        <v>2</v>
+      </c>
+      <c r="T11" s="1">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: horizontal list parser: error message reporting
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372DA76C-6AC2-42C9-B971-BB2D2F8F1224}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677036D1-D38A-4E3C-BE69-2FB86DF31D1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-510" yWindow="8895" windowWidth="38670" windowHeight="15105" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-10635" yWindow="7080" windowWidth="38670" windowHeight="15105" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -870,7 +870,7 @@
   <dimension ref="A1:AD11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: add workbook meta and special @TABLEAU sheet
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677036D1-D38A-4E3C-BE69-2FB86DF31D1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37486F-6713-4402-A0D9-9C23EE93E2AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10635" yWindow="7080" windowWidth="38670" windowHeight="15105" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="4200" yWindow="5355" windowWidth="38670" windowHeight="15105" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
     <sheet name="Reward" sheetId="3" r:id="rId2"/>
+    <sheet name="Exchange" sheetId="7" r:id="rId3"/>
+    <sheet name="@TABLEAU" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -449,6 +451,58 @@
   </si>
   <si>
     <t>DurationDelayedDays</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>NameCellLine</t>
+  </si>
+  <si>
+    <t>TypeCellLine</t>
+  </si>
+  <si>
+    <t>ActivityInfo</t>
+  </si>
+  <si>
+    <t>Exchange</t>
+  </si>
+  <si>
+    <t>ExchangeInfo</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>award1</t>
+  </si>
+  <si>
+    <t>id
+ID</t>
+  </si>
+  <si>
+    <t>INTEGER
+map&lt;uint32, Reward&gt;</t>
+  </si>
+  <si>
+    <t>VARCHAR(64)
+string</t>
+  </si>
+  <si>
+    <t>desc
+Desc</t>
+  </si>
+  <si>
+    <t>award2</t>
   </si>
 </sst>
 </file>
@@ -526,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -553,6 +607,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -869,8 +926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -902,7 +959,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -1660,7 +1717,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2016,4 +2073,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F9FD80-3C33-41B7-9645-F86234050109}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" customWidth="1"/>
+    <col min="2" max="2" width="13.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="12.375" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: support datetime, date, and time
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F37486F-6713-4402-A0D9-9C23EE93E2AF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5235103F-7B7E-46ED-A274-C025C4B91F8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="5355" windowWidth="38670" windowHeight="15105" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="8085" yWindow="9450" windowWidth="38670" windowHeight="15105" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -183,9 +183,6 @@
     <t>SectionItem3Num</t>
   </si>
   <si>
-    <t>timestamp</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
@@ -475,12 +472,6 @@
   </si>
   <si>
     <t>ExchangeInfo</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>date</t>
   </si>
   <si>
     <t>award1</t>
@@ -503,6 +494,51 @@
   </si>
   <si>
     <t>award2</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>begin_time
+BeginTime</t>
+  </si>
+  <si>
+    <t>datetime
+datetime</t>
+  </si>
+  <si>
+    <t>Date
+Date</t>
+  </si>
+  <si>
+    <t>date
+date</t>
+  </si>
+  <si>
+    <t>2020-01-01</t>
+  </si>
+  <si>
+    <t>Time
+Time</t>
+  </si>
+  <si>
+    <t>time
+time</t>
+  </si>
+  <si>
+    <t>日期</t>
+  </si>
+  <si>
+    <t>时间</t>
+  </si>
+  <si>
+    <t>award3</t>
+  </si>
+  <si>
+    <t>20200101</t>
+  </si>
+  <si>
+    <t>050000</t>
   </si>
 </sst>
 </file>
@@ -544,7 +580,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -576,11 +612,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -609,6 +658,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -926,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:AD11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -996,63 +1062,63 @@
         <v>48</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="R1" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>65</v>
-      </c>
       <c r="X1" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AB1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="AD1" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
@@ -1070,70 +1136,70 @@
         <v>34</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="S2" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AC2" s="4" t="s">
         <v>34</v>
@@ -1183,46 +1249,46 @@
         <v>5</v>
       </c>
       <c r="P3" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="R3" s="6" t="s">
         <v>15</v>
       </c>
       <c r="S3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="V3" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="W3" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Y3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Z3" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AA3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AB3" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>79</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1230,7 +1296,7 @@
         <v>100001</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1269,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>17</v>
@@ -1284,10 +1350,10 @@
         <v>10</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Z4" s="1">
         <v>1</v>
@@ -1298,7 +1364,7 @@
         <v>100001</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1339,7 +1405,7 @@
         <v>1</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>17</v>
@@ -1354,10 +1420,10 @@
         <v>10</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="Z5" s="1">
         <v>1</v>
@@ -1368,7 +1434,7 @@
         <v>100001</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1397,7 +1463,7 @@
         <v>5</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>21</v>
@@ -1409,7 +1475,7 @@
         <v>2</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>18</v>
@@ -1424,16 +1490,16 @@
         <v>1</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Z6" s="1">
         <v>1</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1441,7 +1507,7 @@
         <v>100001</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -1462,7 +1528,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>21</v>
@@ -1474,7 +1540,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>18</v>
@@ -1489,16 +1555,16 @@
         <v>1</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1506,7 +1572,7 @@
         <v>100001</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -1531,7 +1597,7 @@
         <v>100001</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1591,7 +1657,7 @@
         <v>100002</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1651,7 +1717,7 @@
         <v>100003</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -1743,116 +1809,116 @@
   <sheetData>
     <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="I2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>29</v>
@@ -1867,25 +1933,25 @@
         <v>27</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>105</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>29</v>
@@ -1905,7 +1971,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1952,7 +2018,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -1999,7 +2065,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -2040,7 +2106,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -2077,69 +2143,125 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F9FD80-3C33-41B7-9645-F86234050109}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="H11" sqref="H10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
+    <col min="3" max="3" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>153</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+      <c r="D1" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>1</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="19">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>2</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>154</v>
+      <c r="C5" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="19">
+        <v>0.20833333333333334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2161,24 +2283,24 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2189,10 +2311,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" t="s">
         <v>145</v>
-      </c>
-      <c r="B3" t="s">
-        <v>146</v>
       </c>
       <c r="C3">
         <v>2</v>

</xml_diff>

<commit_message>
feat: sheet alias name as proto message name
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5235103F-7B7E-46ED-A274-C025C4B91F8F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3425CFC0-9891-40CC-9BC2-CA28925C0361}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8085" yWindow="9450" windowWidth="38670" windowHeight="15105" activeTab="2" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="5160" yWindow="5520" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -463,9 +463,6 @@
   </si>
   <si>
     <t>TypeCellLine</t>
-  </si>
-  <si>
-    <t>ActivityInfo</t>
   </si>
   <si>
     <t>Exchange</t>
@@ -1157,10 +1154,10 @@
         <v>136</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>53</v>
@@ -2145,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F9FD80-3C33-41B7-9645-F86234050109}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H10:H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2159,36 +2156,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>149</v>
-      </c>
       <c r="C2" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2202,10 +2199,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>160</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2213,13 +2210,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E4" s="19">
         <v>0.20833333333333334</v>
@@ -2230,13 +2227,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E5" s="19">
         <v>0.20833333333333334</v>
@@ -2247,16 +2244,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>163</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2269,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2299,9 +2296,6 @@
       <c r="A2" t="s">
         <v>138</v>
       </c>
-      <c r="B2" t="s">
-        <v>143</v>
-      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2311,10 +2305,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
         <v>144</v>
-      </c>
-      <c r="B3" t="s">
-        <v>145</v>
       </c>
       <c r="C3">
         <v>2</v>

</xml_diff>

<commit_message>
feat: support nameline and typeline
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3425CFC0-9891-40CC-9BC2-CA28925C0361}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D911C7F8-47F0-4012-8951-174BC2D657A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="5520" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1575" yWindow="4050" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="164">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -457,12 +457,6 @@
   </si>
   <si>
     <t>Alias</t>
-  </si>
-  <si>
-    <t>NameCellLine</t>
-  </si>
-  <si>
-    <t>TypeCellLine</t>
   </si>
   <si>
     <t>Exchange</t>
@@ -536,6 +530,12 @@
   </si>
   <si>
     <t>050000</t>
+  </si>
+  <si>
+    <t>Nameline</t>
+  </si>
+  <si>
+    <t>Typeline</t>
   </si>
 </sst>
 </file>
@@ -1154,10 +1154,10 @@
         <v>136</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>53</v>
@@ -2156,36 +2156,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>152</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>154</v>
-      </c>
       <c r="E1" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>155</v>
-      </c>
       <c r="E2" s="13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
@@ -2199,10 +2199,10 @@
         <v>4</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2210,13 +2210,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" s="19">
         <v>0.20833333333333334</v>
@@ -2227,13 +2227,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E5" s="19">
         <v>0.20833333333333334</v>
@@ -2244,16 +2244,16 @@
         <v>3</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2286,10 +2286,10 @@
         <v>140</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>141</v>
+        <v>162</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>142</v>
+        <v>163</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2305,10 +2305,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C3">
         <v>2</v>

</xml_diff>

<commit_message>
feat: set nameline and typeline at global config
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D911C7F8-47F0-4012-8951-174BC2D657A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFBB1E-6C72-4113-A63A-8E191679E6AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="4050" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="1410" yWindow="5115" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -2143,7 +2143,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2267,7 +2267,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2311,10 +2311,10 @@
         <v>142</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: support incell list with name index
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69BFBB1E-6C72-4113-A63A-8E191679E6AD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047D7DDA-DC2E-4BD6-9ACB-BC1AC7B7C66A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="5115" windowWidth="38670" windowHeight="15105" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-1905" yWindow="7170" windowWidth="38670" windowHeight="13035" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -536,6 +536,33 @@
   </si>
   <si>
     <t>Typeline</t>
+  </si>
+  <si>
+    <t>TaskParamList1</t>
+  </si>
+  <si>
+    <t>TaskParamList2</t>
+  </si>
+  <si>
+    <t>参数列表1</t>
+  </si>
+  <si>
+    <t>参数列表2</t>
+  </si>
+  <si>
+    <t>4,5,6</t>
+  </si>
+  <si>
+    <t>10,11,12</t>
+  </si>
+  <si>
+    <t>13,14,15</t>
+  </si>
+  <si>
+    <t>TaskParamList3</t>
+  </si>
+  <si>
+    <t>40,50,60</t>
   </si>
 </sst>
 </file>
@@ -626,7 +653,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -672,6 +699,9 @@
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -987,10 +1017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:AD11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1:Y2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1014,14 +1044,16 @@
     <col min="18" max="18" width="9.75" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="16.25" customWidth="1"/>
-    <col min="28" max="30" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.75" customWidth="1"/>
+    <col min="24" max="25" width="15.875" customWidth="1"/>
+    <col min="26" max="26" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.25" customWidth="1"/>
+    <col min="31" max="33" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -1089,31 +1121,40 @@
         <v>63</v>
       </c>
       <c r="W1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -1181,31 +1222,40 @@
         <v>53</v>
       </c>
       <c r="W2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="Z2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="AA2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1267,28 +1317,37 @@
         <v>60</v>
       </c>
       <c r="W3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="X3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="Y3" s="6" t="s">
+      <c r="AB3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="AC3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1343,20 +1402,20 @@
       <c r="T4" s="1">
         <v>1</v>
       </c>
-      <c r="W4" s="1">
+      <c r="Z4" s="1">
         <v>10</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="AA4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Z4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1413,20 +1472,29 @@
       <c r="T5" s="1">
         <v>1</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Z5" s="1">
         <v>10</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="AA5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="Z5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AC5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1483,23 +1551,32 @@
       <c r="T6" s="1">
         <v>2</v>
       </c>
-      <c r="W6" s="1">
-        <v>1</v>
+      <c r="W6" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="X6" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Y6" s="20">
+        <v>130140150</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="Z6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AC6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1548,23 +1625,23 @@
       <c r="T7" s="1">
         <v>3</v>
       </c>
-      <c r="W7" s="1">
-        <v>1</v>
-      </c>
-      <c r="X7" s="1" t="s">
+      <c r="Z7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1589,7 +1666,7 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100001</v>
       </c>
@@ -1649,7 +1726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100002</v>
       </c>
@@ -1709,7 +1786,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:30" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>100003</v>
       </c>
@@ -2266,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
feat(protogen): support nested naming of name row
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047D7DDA-DC2E-4BD6-9ACB-BC1AC7B7C66A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4ECD2-D5F1-4746-8215-BED7F2EAD14B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1905" yWindow="7170" windowWidth="38670" windowHeight="13035" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="2145" yWindow="3030" windowWidth="36225" windowHeight="13035" activeTab="5" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
     <sheet name="Reward" sheetId="3" r:id="rId2"/>
     <sheet name="Exchange" sheetId="7" r:id="rId3"/>
-    <sheet name="@TABLEAU" sheetId="4" r:id="rId4"/>
+    <sheet name="Match" sheetId="8" r:id="rId4"/>
+    <sheet name="@TABLEAU" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="209">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -563,6 +565,114 @@
   </si>
   <si>
     <t>40,50,60</t>
+  </si>
+  <si>
+    <t>Match</t>
+  </si>
+  <si>
+    <t>MatchConf</t>
+  </si>
+  <si>
+    <t>Nested</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>map&lt;uint32, Mode&gt;</t>
+  </si>
+  <si>
+    <t>Timeout</t>
+  </si>
+  <si>
+    <t>超时时间</t>
+  </si>
+  <si>
+    <t>ModeID</t>
+  </si>
+  <si>
+    <t>ModeDesc</t>
+  </si>
+  <si>
+    <t>mode1</t>
+  </si>
+  <si>
+    <t>mode2</t>
+  </si>
+  <si>
+    <t>mode3</t>
+  </si>
+  <si>
+    <t>TaskFilterType</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>TaskFilterOpen</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>间隔时间</t>
+  </si>
+  <si>
+    <t>ModeDifficulty</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionID</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionName</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionItem1Id</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionItem1Num</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionItem2Id</t>
+  </si>
+  <si>
+    <t>TaskFilterSectionItem2Num</t>
+  </si>
+  <si>
+    <t>RobotType</t>
+  </si>
+  <si>
+    <t>{Robot}int32</t>
+  </si>
+  <si>
+    <t>RobotAbility</t>
+  </si>
+  <si>
+    <t>机器人类型</t>
+  </si>
+  <si>
+    <t>{AI}int32</t>
+  </si>
+  <si>
+    <t>AI类型</t>
+  </si>
+  <si>
+    <t>能力</t>
+  </si>
+  <si>
+    <t>ModeAIType</t>
+  </si>
+  <si>
+    <t>ModeAIAbility</t>
+  </si>
+  <si>
+    <t>过滤器类型</t>
+  </si>
+  <si>
+    <t>过滤器是否打开</t>
+  </si>
+  <si>
+    <t>map&lt;uint32,Filter&gt;</t>
   </si>
 </sst>
 </file>
@@ -653,7 +763,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -702,6 +812,25 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1019,8 +1148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:Y2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2220,7 +2349,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2340,11 +2469,406 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098EE3E-D65B-4BEF-90E6-B8EB44A5D5DA}">
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="8.875" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="27" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="12.625" customWidth="1"/>
+    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.25" customWidth="1"/>
+    <col min="12" max="12" width="15.375" customWidth="1"/>
+    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.25" customWidth="1"/>
+    <col min="20" max="20" width="10.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>181</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>179</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="26">
+        <v>1</v>
+      </c>
+      <c r="B4" s="26">
+        <v>11</v>
+      </c>
+      <c r="C4" s="26">
+        <v>1</v>
+      </c>
+      <c r="D4" s="26">
+        <v>11</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>9</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <v>1</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O4" s="2">
+        <v>2001</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="1">
+        <v>8</v>
+      </c>
+      <c r="T4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
+        <v>2</v>
+      </c>
+      <c r="B5" s="26">
+        <v>12</v>
+      </c>
+      <c r="C5" s="26">
+        <v>2</v>
+      </c>
+      <c r="D5" s="26">
+        <v>12</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9</v>
+      </c>
+      <c r="G5" s="1">
+        <v>4</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9</v>
+      </c>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
+      <c r="J5" s="1">
+        <v>5</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O5" s="2">
+        <v>2002</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="1">
+        <v>9</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="26">
+        <v>3</v>
+      </c>
+      <c r="B6" s="26">
+        <v>13</v>
+      </c>
+      <c r="C6" s="26">
+        <v>3</v>
+      </c>
+      <c r="D6" s="26">
+        <v>13</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1">
+        <v>7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
+        <v>3</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O6" s="2">
+        <v>2003</v>
+      </c>
+      <c r="P6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>2005</v>
+      </c>
+      <c r="R6" s="2">
+        <v>14</v>
+      </c>
+      <c r="S6" s="1">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2879,7 @@
     <col min="4" max="4" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -2368,8 +2892,11 @@
       <c r="D1" s="4" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -2380,7 +2907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -2392,6 +2919,84 @@
       </c>
       <c r="D3">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998E967-D8C7-4603-9CFE-5D9ECC3EE6B0}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat(protogen): support horizontal map and more smart incell map
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87A4ECD2-D5F1-4746-8215-BED7F2EAD14B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F698F72B-1959-4B02-9C91-C313BC00F47D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="3030" windowWidth="36225" windowHeight="13035" activeTab="5" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-1605" yWindow="7410" windowWidth="36225" windowHeight="13035" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="223">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -673,6 +673,48 @@
   </si>
   <si>
     <t>map&lt;uint32,Filter&gt;</t>
+  </si>
+  <si>
+    <t>因子类型</t>
+  </si>
+  <si>
+    <t>因子值</t>
+  </si>
+  <si>
+    <t>Factor1Type</t>
+  </si>
+  <si>
+    <t>Factor2Value</t>
+  </si>
+  <si>
+    <t>Factor2Type</t>
+  </si>
+  <si>
+    <t>Factor1Value</t>
+  </si>
+  <si>
+    <t>map&lt;int32, Factor&gt;</t>
+  </si>
+  <si>
+    <t>TaskParamMap1</t>
+  </si>
+  <si>
+    <t>map&lt;int32, int32&gt;</t>
+  </si>
+  <si>
+    <t>1:2,3:4</t>
+  </si>
+  <si>
+    <t>5:6,7:8</t>
+  </si>
+  <si>
+    <t>TaskParamMap2</t>
+  </si>
+  <si>
+    <t>10:20,30:40</t>
+  </si>
+  <si>
+    <t>50:60,70:80</t>
   </si>
 </sst>
 </file>
@@ -763,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -831,6 +873,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1146,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
-  <dimension ref="A1:AG11"/>
+  <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1174,15 +1219,15 @@
     <col min="19" max="19" width="10" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="10.75" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14.75" customWidth="1"/>
-    <col min="24" max="25" width="15.875" customWidth="1"/>
-    <col min="26" max="26" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="31.375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.25" customWidth="1"/>
-    <col min="31" max="33" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="15.875" customWidth="1"/>
+    <col min="28" max="28" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="31.375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.25" customWidth="1"/>
+    <col min="33" max="35" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -1259,31 +1304,37 @@
         <v>171</v>
       </c>
       <c r="Z1" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -1360,31 +1411,37 @@
         <v>109</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>53</v>
+        <v>217</v>
       </c>
       <c r="AA2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AC2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1455,28 +1512,34 @@
         <v>167</v>
       </c>
       <c r="Z3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB3" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="AB3" s="6" t="s">
+      <c r="AD3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AE3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="AD3" s="6" t="s">
+      <c r="AF3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AE3" s="6" t="s">
+      <c r="AG3" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="AF3" s="6" t="s">
+      <c r="AH3" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="AG3" s="6" t="s">
+      <c r="AI3" s="6" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1531,20 +1594,20 @@
       <c r="T4" s="1">
         <v>1</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="AB4" s="1">
         <v>10</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AC4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1610,20 +1673,26 @@
       <c r="Y5" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="Z5" s="1">
+      <c r="Z5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AB5" s="1">
         <v>10</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AC5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1689,23 +1758,29 @@
       <c r="Y6" s="20">
         <v>130140150</v>
       </c>
-      <c r="Z6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="Z6" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="AA6" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="AC6" s="1">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AE6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1754,23 +1829,23 @@
       <c r="T7" s="1">
         <v>3</v>
       </c>
-      <c r="Z7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AE7" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AF7" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1795,7 +1870,7 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100001</v>
       </c>
@@ -1855,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100002</v>
       </c>
@@ -1915,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:33" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>100003</v>
       </c>
@@ -2470,10 +2545,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098EE3E-D65B-4BEF-90E6-B8EB44A5D5DA}">
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2481,24 +2556,28 @@
     <col min="1" max="2" width="8.875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="27" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.25" customWidth="1"/>
-    <col min="7" max="7" width="12.625" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.25" customWidth="1"/>
-    <col min="12" max="12" width="15.375" customWidth="1"/>
-    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.25" customWidth="1"/>
-    <col min="20" max="20" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="27" customWidth="1"/>
+    <col min="7" max="7" width="17.375" style="27" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" style="27" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.25" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.25" customWidth="1"/>
+    <col min="16" max="16" width="15.375" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.25" customWidth="1"/>
+    <col min="24" max="24" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>188</v>
       </c>
@@ -2506,61 +2585,73 @@
         <v>178</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>214</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="H1" s="23" t="s">
         <v>190</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="I1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="L1" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="M1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="N1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="O1" s="28" t="s">
         <v>185</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="P1" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="Q1" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="R1" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="S1" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="T1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="V1" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="W1" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="X1" s="28" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>53</v>
       </c>
@@ -2568,61 +2659,73 @@
         <v>53</v>
       </c>
       <c r="C2" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="D2" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="H2" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="J2" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="K2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="M2" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="4" t="s">
+      <c r="N2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="P2" s="28" t="s">
         <v>186</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="Q2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="R2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="S2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" s="4" t="s">
+      <c r="T2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="W2" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="T2" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>189</v>
       </c>
@@ -2630,61 +2733,73 @@
         <v>179</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="G3" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="H3" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="K3" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="L3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="M3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="S3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>1</v>
       </c>
@@ -2692,55 +2807,67 @@
         <v>11</v>
       </c>
       <c r="C4" s="26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D4" s="26">
         <v>11</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="26">
+        <v>100</v>
+      </c>
+      <c r="F4" s="26">
+        <v>11</v>
+      </c>
+      <c r="G4" s="26">
+        <v>1</v>
+      </c>
+      <c r="H4" s="26">
+        <v>11</v>
+      </c>
+      <c r="I4" s="26" t="s">
         <v>182</v>
       </c>
-      <c r="F4" s="1">
+      <c r="J4" s="1">
         <v>8</v>
       </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-      <c r="H4" s="1">
+      <c r="K4" s="1">
+        <v>1</v>
+      </c>
+      <c r="L4" s="1">
         <v>9</v>
       </c>
-      <c r="I4" s="1">
-        <v>1</v>
-      </c>
-      <c r="J4" s="1">
-        <v>2</v>
-      </c>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1"/>
       <c r="M4" s="1">
         <v>1</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="1">
+        <v>2</v>
+      </c>
+      <c r="O4" s="1">
+        <v>1</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1">
+        <v>1</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="2">
+      <c r="S4" s="2">
         <v>2001</v>
       </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="1">
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="1">
         <v>8</v>
       </c>
-      <c r="T4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="X4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="26">
         <v>2</v>
       </c>
@@ -2748,55 +2875,67 @@
         <v>12</v>
       </c>
       <c r="C5" s="26">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D5" s="26">
         <v>12</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="26">
+        <v>200</v>
+      </c>
+      <c r="F5" s="26">
+        <v>12</v>
+      </c>
+      <c r="G5" s="26">
+        <v>2</v>
+      </c>
+      <c r="H5" s="26">
+        <v>12</v>
+      </c>
+      <c r="I5" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="F5" s="1">
+      <c r="J5" s="1">
         <v>9</v>
       </c>
-      <c r="G5" s="1">
+      <c r="K5" s="1">
         <v>4</v>
       </c>
-      <c r="H5" s="1">
+      <c r="L5" s="1">
         <v>9</v>
       </c>
-      <c r="I5" s="1">
+      <c r="M5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
+      <c r="N5" s="1">
         <v>5</v>
       </c>
-      <c r="K5" s="1">
-        <v>2</v>
-      </c>
-      <c r="L5" s="3"/>
-      <c r="M5" s="1">
-        <v>2</v>
-      </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1">
+        <v>2</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="1">
+        <v>2</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="2">
+      <c r="S5" s="2">
         <v>2002</v>
       </c>
-      <c r="P5" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="1">
+      <c r="T5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="1">
         <v>9</v>
       </c>
-      <c r="T5" s="1">
+      <c r="X5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>3</v>
       </c>
@@ -2804,57 +2943,69 @@
         <v>13</v>
       </c>
       <c r="C6" s="26">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D6" s="26">
         <v>13</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="26">
+        <v>300</v>
+      </c>
+      <c r="F6" s="26">
+        <v>13</v>
+      </c>
+      <c r="G6" s="26">
+        <v>3</v>
+      </c>
+      <c r="H6" s="26">
+        <v>13</v>
+      </c>
+      <c r="I6" s="26" t="s">
         <v>184</v>
       </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
+      <c r="J6" s="1">
+        <v>1</v>
+      </c>
+      <c r="K6" s="1">
         <v>7</v>
       </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="L6" s="1">
+        <v>1</v>
+      </c>
+      <c r="M6" s="1">
         <v>7</v>
       </c>
-      <c r="J6" s="1">
+      <c r="N6" s="1">
         <v>8</v>
       </c>
-      <c r="K6" s="1">
+      <c r="O6" s="1">
         <v>3</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="P6" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="M6" s="1">
+      <c r="Q6" s="1">
         <v>3</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O6" s="2">
+      <c r="S6" s="2">
         <v>2003</v>
       </c>
-      <c r="P6" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="2">
+      <c r="T6" s="2">
+        <v>2</v>
+      </c>
+      <c r="U6" s="2">
         <v>2005</v>
       </c>
-      <c r="R6" s="2">
+      <c r="V6" s="2">
         <v>14</v>
       </c>
-      <c r="S6" s="1">
-        <v>1</v>
-      </c>
-      <c r="T6" s="1">
+      <c r="W6" s="1">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1">
         <v>7</v>
       </c>
     </row>
@@ -2865,10 +3016,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2921,6 +3072,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -2931,8 +3099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998E967-D8C7-4603-9CFE-5D9ECC3EE6B0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat(protogen): support nested composite types: map, list, and struct
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F698F72B-1959-4B02-9C91-C313BC00F47D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A44A7-EFF8-4AD9-8D6C-08BF21509EDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1605" yWindow="7410" windowWidth="36225" windowHeight="13035" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-13755" yWindow="3120" windowWidth="48630" windowHeight="11910" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="229">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -651,9 +651,6 @@
     <t>机器人类型</t>
   </si>
   <si>
-    <t>{AI}int32</t>
-  </si>
-  <si>
     <t>AI类型</t>
   </si>
   <si>
@@ -715,6 +712,27 @@
   </si>
   <si>
     <t>50:60,70:80</t>
+  </si>
+  <si>
+    <t>难度</t>
+  </si>
+  <si>
+    <t>mode4</t>
+  </si>
+  <si>
+    <t>签到活动节4</t>
+  </si>
+  <si>
+    <t>[AI]int32</t>
+  </si>
+  <si>
+    <t>[Job]int32</t>
+  </si>
+  <si>
+    <t>TaskFilterJobType</t>
+  </si>
+  <si>
+    <t>TaskFilterJobCount</t>
   </si>
 </sst>
 </file>
@@ -730,7 +748,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,6 +770,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -805,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -876,6 +900,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1193,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EB9BCC5-DC51-4147-998A-9AFD936B0F72}">
   <dimension ref="A1:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="AA12" sqref="AA12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1304,10 +1337,10 @@
         <v>171</v>
       </c>
       <c r="Z1" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AA1" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>64</v>
@@ -1411,10 +1444,10 @@
         <v>109</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AB2" s="4" t="s">
         <v>53</v>
@@ -1674,10 +1707,10 @@
         <v>172</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AB5" s="1">
         <v>10</v>
@@ -1759,10 +1792,10 @@
         <v>130140150</v>
       </c>
       <c r="Z6" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AA6" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="AB6" s="1">
         <v>1</v>
@@ -2545,10 +2578,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098EE3E-D65B-4BEF-90E6-B8EB44A5D5DA}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2567,17 +2600,19 @@
     <col min="13" max="14" width="10.75" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.25" customWidth="1"/>
     <col min="16" max="16" width="15.375" customWidth="1"/>
-    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.625" customWidth="1"/>
+    <col min="18" max="18" width="18.25" customWidth="1"/>
+    <col min="19" max="19" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="23.375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.25" customWidth="1"/>
-    <col min="24" max="24" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.25" customWidth="1"/>
+    <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>188</v>
       </c>
@@ -2585,16 +2620,16 @@
         <v>178</v>
       </c>
       <c r="C1" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>212</v>
+      </c>
+      <c r="F1" s="23" t="s">
         <v>211</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>214</v>
-      </c>
-      <c r="E1" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="F1" s="23" t="s">
-        <v>212</v>
       </c>
       <c r="G1" s="23" t="s">
         <v>180</v>
@@ -2606,10 +2641,10 @@
         <v>181</v>
       </c>
       <c r="J1" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" s="28" t="s">
         <v>204</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>205</v>
       </c>
       <c r="L1" s="28" t="s">
         <v>56</v>
@@ -2627,31 +2662,37 @@
         <v>187</v>
       </c>
       <c r="Q1" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="S1" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>193</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>195</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>196</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>53</v>
       </c>
@@ -2659,7 +2700,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D2" s="24" t="s">
         <v>53</v>
@@ -2680,7 +2721,7 @@
         <v>34</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
       <c r="K2" s="28" t="s">
         <v>53</v>
@@ -2695,37 +2736,43 @@
         <v>53</v>
       </c>
       <c r="O2" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="P2" s="28" t="s">
         <v>186</v>
       </c>
       <c r="Q2" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="R2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="T2" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="U2" s="28" t="s">
         <v>55</v>
-      </c>
-      <c r="T2" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>53</v>
       </c>
       <c r="V2" s="28" t="s">
         <v>53</v>
       </c>
       <c r="W2" s="28" t="s">
-        <v>198</v>
+        <v>53</v>
       </c>
       <c r="X2" s="28" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:24" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Y2" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z2" s="28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>189</v>
       </c>
@@ -2733,31 +2780,31 @@
         <v>179</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="D3" s="25" t="s">
-        <v>210</v>
-      </c>
       <c r="E3" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>209</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>210</v>
       </c>
       <c r="G3" s="25" t="s">
         <v>69</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>71</v>
+        <v>222</v>
       </c>
       <c r="I3" s="25" t="s">
         <v>71</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>57</v>
@@ -2769,37 +2816,43 @@
         <v>59</v>
       </c>
       <c r="O3" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="P3" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="P3" s="6" t="s">
-        <v>207</v>
-      </c>
       <c r="Q3" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="V3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="U3" s="6" t="s">
+      <c r="W3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="6" t="s">
+      <c r="X3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="W3" s="6" t="s">
+      <c r="Y3" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="X3" s="6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Z3" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>1</v>
       </c>
@@ -2828,13 +2881,13 @@
         <v>182</v>
       </c>
       <c r="J4" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="K4" s="1">
         <v>1</v>
       </c>
       <c r="L4" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M4" s="1">
         <v>1</v>
@@ -2849,93 +2902,105 @@
       <c r="Q4" s="1">
         <v>1</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="1">
+        <v>1</v>
+      </c>
+      <c r="S4" s="1">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="S4" s="2">
+      <c r="U4" s="2">
         <v>2001</v>
       </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="1">
-        <v>8</v>
-      </c>
-      <c r="X4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="26">
-        <v>2</v>
-      </c>
-      <c r="B5" s="26">
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>2</v>
+      </c>
+      <c r="B5" s="29">
         <v>12</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="29">
         <v>20</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="29">
         <v>12</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="29">
         <v>200</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="29">
         <v>12</v>
       </c>
-      <c r="G5" s="26">
-        <v>2</v>
-      </c>
-      <c r="H5" s="26">
+      <c r="G5" s="29">
+        <v>2</v>
+      </c>
+      <c r="H5" s="29">
         <v>12</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="J5" s="1">
-        <v>9</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="J5" s="30">
+        <v>2</v>
+      </c>
+      <c r="K5" s="30">
         <v>4</v>
       </c>
-      <c r="L5" s="1">
-        <v>9</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="L5" s="30">
+        <v>2</v>
+      </c>
+      <c r="M5" s="30">
+        <v>2</v>
+      </c>
+      <c r="N5" s="30">
+        <v>5</v>
+      </c>
+      <c r="O5" s="30">
+        <v>2</v>
+      </c>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="30">
+        <v>2</v>
+      </c>
+      <c r="R5" s="30">
         <v>4</v>
       </c>
-      <c r="N5" s="1">
-        <v>5</v>
-      </c>
-      <c r="O5" s="1">
-        <v>2</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="1">
-        <v>2</v>
-      </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="30">
+        <v>2</v>
+      </c>
+      <c r="T5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="2">
+      <c r="U5" s="30">
         <v>2002</v>
       </c>
-      <c r="T5" s="2">
-        <v>1</v>
-      </c>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="1">
-        <v>9</v>
-      </c>
-      <c r="X5" s="1">
+      <c r="V5" s="30">
+        <v>2</v>
+      </c>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="30">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>3</v>
       </c>
@@ -2954,59 +3019,145 @@
       <c r="F6" s="26">
         <v>13</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="29">
         <v>3</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="29">
         <v>13</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="J6" s="1">
-        <v>1</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="J6" s="30">
+        <v>3</v>
+      </c>
+      <c r="K6" s="30">
         <v>7</v>
       </c>
       <c r="L6" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M6" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="N6" s="1">
         <v>8</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="30">
         <v>3</v>
       </c>
-      <c r="P6" s="3" t="s">
+      <c r="P6" s="31" t="s">
         <v>176</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="Q6" s="30">
         <v>3</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="30">
+        <v>7</v>
+      </c>
+      <c r="S6" s="30">
+        <v>3</v>
+      </c>
+      <c r="T6" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="S6" s="2">
+      <c r="U6" s="30">
         <v>2003</v>
       </c>
-      <c r="T6" s="2">
-        <v>2</v>
-      </c>
-      <c r="U6" s="2">
+      <c r="V6" s="30">
+        <v>3</v>
+      </c>
+      <c r="W6" s="30">
         <v>2005</v>
       </c>
-      <c r="V6" s="2">
+      <c r="X6" s="30">
+        <v>13</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="26">
+        <v>4</v>
+      </c>
+      <c r="B7" s="26">
         <v>14</v>
       </c>
-      <c r="W6" s="1">
-        <v>1</v>
-      </c>
-      <c r="X6" s="1">
+      <c r="C7" s="26">
+        <v>30</v>
+      </c>
+      <c r="D7" s="26">
+        <v>14</v>
+      </c>
+      <c r="E7" s="26">
+        <v>300</v>
+      </c>
+      <c r="F7" s="26">
+        <v>14</v>
+      </c>
+      <c r="G7" s="29">
+        <v>3</v>
+      </c>
+      <c r="H7" s="29">
+        <v>14</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="J7" s="30">
+        <v>4</v>
+      </c>
+      <c r="K7" s="30">
         <v>7</v>
+      </c>
+      <c r="L7" s="1">
+        <v>4</v>
+      </c>
+      <c r="M7" s="1">
+        <v>4</v>
+      </c>
+      <c r="N7" s="1">
+        <v>8</v>
+      </c>
+      <c r="O7" s="30">
+        <v>3</v>
+      </c>
+      <c r="P7" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>4</v>
+      </c>
+      <c r="R7" s="30">
+        <v>7</v>
+      </c>
+      <c r="S7" s="30">
+        <v>4</v>
+      </c>
+      <c r="T7" s="30" t="s">
+        <v>224</v>
+      </c>
+      <c r="U7" s="30">
+        <v>2004</v>
+      </c>
+      <c r="V7" s="30">
+        <v>4</v>
+      </c>
+      <c r="W7" s="30">
+        <v>2005</v>
+      </c>
+      <c r="X7" s="30">
+        <v>14</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>4</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feature: auto-populate the missing map key for easy use and clear reading
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{480A44A7-EFF8-4AD9-8D6C-08BF21509EDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A783FC-641D-45DE-BBEA-953284AA2DF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13755" yWindow="3120" windowWidth="48630" windowHeight="11910" activeTab="3" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="330" yWindow="3180" windowWidth="48630" windowHeight="16695" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
     <sheet name="Reward" sheetId="3" r:id="rId2"/>
     <sheet name="Exchange" sheetId="7" r:id="rId3"/>
     <sheet name="Match" sheetId="8" r:id="rId4"/>
-    <sheet name="@TABLEAU" sheetId="4" r:id="rId5"/>
-    <sheet name="Sheet2" sheetId="9" r:id="rId6"/>
+    <sheet name="Loader" sheetId="10" r:id="rId5"/>
+    <sheet name="@TABLEAU" sheetId="4" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,44 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>youngerli(李飞洋)</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{43698F2A-FC46-4A56-89B7-D11A72E1A6E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>youngerli(李飞洋):</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+Excel的Sheet名称</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="245">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -733,13 +770,67 @@
   </si>
   <si>
     <t>TaskFilterJobCount</t>
+  </si>
+  <si>
+    <t>ServerName</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>ServerConfName</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>map&lt;string, Server&gt;</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>[Conf]string</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>进程名</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置列表</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Loader</t>
+  </si>
+  <si>
+    <t>matchsvr</t>
+  </si>
+  <si>
+    <t>gamesvr</t>
+  </si>
+  <si>
+    <t>HeadFrameConf</t>
+  </si>
+  <si>
+    <t>activitysvr</t>
+  </si>
+  <si>
+    <t>ActivityConf</t>
+  </si>
+  <si>
+    <t>ChapterConf</t>
+  </si>
+  <si>
+    <t>CollectionConf</t>
+  </si>
+  <si>
+    <t>ExchangeConf</t>
+  </si>
+  <si>
+    <t>SectionConf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -747,8 +838,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -779,8 +894,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -825,11 +946,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -908,6 +1057,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1230,7 +1385,7 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
@@ -1260,7 +1415,7 @@
     <col min="33" max="35" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="4" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -1367,7 +1522,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -1474,7 +1629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" s="6" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1572,7 +1727,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" s="1" customFormat="1">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1640,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" s="1" customFormat="1">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1725,7 +1880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" s="1" customFormat="1">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1813,7 +1968,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -1878,7 +2033,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -1903,7 +2058,7 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>100001</v>
       </c>
@@ -1963,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>100002</v>
       </c>
@@ -2023,7 +2178,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>100003</v>
       </c>
@@ -2097,7 +2252,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
@@ -2118,7 +2273,7 @@
     <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="8" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
@@ -2171,7 +2326,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" s="8" customFormat="1">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -2224,7 +2379,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
@@ -2277,7 +2432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2324,7 +2479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2371,7 +2526,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2412,7 +2567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2457,10 +2612,10 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -2468,7 +2623,7 @@
     <col min="4" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.5">
       <c r="A1" s="12" t="s">
         <v>144</v>
       </c>
@@ -2485,7 +2640,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="31.5">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -2502,7 +2657,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="16" customFormat="1">
       <c r="A3" s="14" t="s">
         <v>69</v>
       </c>
@@ -2519,7 +2674,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -2536,7 +2691,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -2553,7 +2708,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -2580,11 +2735,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8098EE3E-D65B-4BEF-90E6-B8EB44A5D5DA}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="2" width="8.875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="27" bestFit="1" customWidth="1"/>
@@ -2612,7 +2767,7 @@
     <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="22" customFormat="1">
       <c r="A1" s="23" t="s">
         <v>188</v>
       </c>
@@ -2692,7 +2847,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" s="22" customFormat="1">
       <c r="A2" s="24" t="s">
         <v>53</v>
       </c>
@@ -2772,7 +2927,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" s="16" customFormat="1">
       <c r="A3" s="25" t="s">
         <v>189</v>
       </c>
@@ -2852,7 +3007,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26">
       <c r="A4" s="26">
         <v>1</v>
       </c>
@@ -2926,7 +3081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -3000,7 +3155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26">
       <c r="A6" s="26">
         <v>3</v>
       </c>
@@ -3080,7 +3235,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26">
       <c r="A7" s="26">
         <v>4</v>
       </c>
@@ -3166,14 +3321,107 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276FCC3A-35D5-42B7-A495-66FF10558F19}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>237</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>236</v>
+      </c>
+      <c r="B11" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50122103-18AD-494A-9F48-C5E57158EC4A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="10.125" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
@@ -3181,7 +3429,7 @@
     <col min="4" max="4" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -3198,7 +3446,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3209,7 +3457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -3223,7 +3471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3237,6 +3485,20 @@
         <v>1</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>176</v>
       </c>
     </row>
@@ -3246,20 +3508,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998E967-D8C7-4603-9CFE-5D9ECC3EE6B0}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -3276,7 +3538,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3287,7 +3549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -3301,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3315,6 +3577,20 @@
         <v>1</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>176</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: support keyed list, e.g: [Type]<int32>
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A783FC-641D-45DE-BBEA-953284AA2DF0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF067D70-BD8E-4417-AC8F-C6B115A2E5AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="330" yWindow="3180" windowWidth="48630" windowHeight="16695" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="5370" yWindow="5070" windowWidth="24840" windowHeight="13740" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -36,44 +36,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>youngerli(李飞洋)</author>
-  </authors>
-  <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{43698F2A-FC46-4A56-89B7-D11A72E1A6E5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t>youngerli(李飞洋):</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <family val="3"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-Excel的Sheet名称</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="250">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -780,22 +744,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>map&lt;string, Server&gt;</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
-    <t>[Conf]string</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>进程名</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>配置列表</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Loader</t>
   </si>
   <si>
@@ -824,13 +776,37 @@
   </si>
   <si>
     <t>SectionConf</t>
+  </si>
+  <si>
+    <t>配置Sheet名</t>
+  </si>
+  <si>
+    <t>ServerConfConditionType</t>
+  </si>
+  <si>
+    <t>ServerConfConditionValue</t>
+  </si>
+  <si>
+    <t>条件类型</t>
+  </si>
+  <si>
+    <t>条件值</t>
+  </si>
+  <si>
+    <t>[Conf]&lt;string&gt;</t>
+  </si>
+  <si>
+    <t>map&lt;string, Server&gt;</t>
+  </si>
+  <si>
+    <t>[Condition]int32</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -839,28 +815,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="3"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="7">
@@ -978,7 +937,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1065,6 +1024,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1385,7 +1345,7 @@
       <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
@@ -1415,7 +1375,7 @@
     <col min="33" max="35" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="4" customFormat="1">
+    <row r="1" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>32</v>
       </c>
@@ -1522,7 +1482,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:35" s="4" customFormat="1">
+    <row r="2" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>54</v>
       </c>
@@ -1629,7 +1589,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:35" s="6" customFormat="1">
+    <row r="3" spans="1:35" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
@@ -1727,7 +1687,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:35" s="1" customFormat="1">
+    <row r="4" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>100001</v>
       </c>
@@ -1795,7 +1755,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:35" s="1" customFormat="1">
+    <row r="5" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100001</v>
       </c>
@@ -1880,7 +1840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:35" s="1" customFormat="1">
+    <row r="6" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>100001</v>
       </c>
@@ -1968,7 +1928,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:35" s="1" customFormat="1">
+    <row r="7" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>100001</v>
       </c>
@@ -2033,7 +1993,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:35" s="1" customFormat="1">
+    <row r="8" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>100001</v>
       </c>
@@ -2058,7 +2018,7 @@
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
     </row>
-    <row r="9" spans="1:35" s="1" customFormat="1">
+    <row r="9" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>100001</v>
       </c>
@@ -2118,7 +2078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:35" s="1" customFormat="1">
+    <row r="10" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>100002</v>
       </c>
@@ -2178,7 +2138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:35" s="1" customFormat="1">
+    <row r="11" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>100003</v>
       </c>
@@ -2252,7 +2212,7 @@
       <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" bestFit="1" customWidth="1"/>
@@ -2273,7 +2233,7 @@
     <col min="17" max="17" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="8" customFormat="1">
+    <row r="1" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
@@ -2326,7 +2286,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1">
+    <row r="2" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -2379,7 +2339,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1">
+    <row r="3" spans="1:17" s="11" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>69</v>
       </c>
@@ -2432,7 +2392,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2479,7 +2439,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2526,7 +2486,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -2567,7 +2527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -2615,7 +2575,7 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
     <col min="2" max="2" width="13.75" customWidth="1"/>
@@ -2623,7 +2583,7 @@
     <col min="4" max="4" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31.5">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>144</v>
       </c>
@@ -2640,7 +2600,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="31.5">
+    <row r="2" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>145</v>
       </c>
@@ -2657,7 +2617,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="16" customFormat="1">
+    <row r="3" spans="1:5" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>69</v>
       </c>
@@ -2674,7 +2634,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="18">
         <v>1</v>
       </c>
@@ -2691,7 +2651,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>2</v>
       </c>
@@ -2708,7 +2668,7 @@
         <v>0.20833333333333334</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="18">
         <v>3</v>
       </c>
@@ -2739,7 +2699,7 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="8.875" style="27" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.375" style="27" bestFit="1" customWidth="1"/>
@@ -2767,7 +2727,7 @@
     <col min="26" max="26" width="10.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="22" customFormat="1">
+    <row r="1" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>188</v>
       </c>
@@ -2847,7 +2807,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:26" s="22" customFormat="1">
+    <row r="2" spans="1:26" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>53</v>
       </c>
@@ -2927,7 +2887,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="16" customFormat="1">
+    <row r="3" spans="1:26" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>189</v>
       </c>
@@ -3007,7 +2967,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="26">
         <v>1</v>
       </c>
@@ -3081,7 +3041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="29">
         <v>2</v>
       </c>
@@ -3155,7 +3115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="26">
         <v>3</v>
       </c>
@@ -3235,7 +3195,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:26">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="26">
         <v>4</v>
       </c>
@@ -3321,95 +3281,147 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276FCC3A-35D5-42B7-A495-66FF10558F19}">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276FCC3A-35D5-42B7-A495-66FF10558F19}">
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.25" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="28.375" style="34" customWidth="1"/>
+    <col min="4" max="4" width="22.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>229</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="32" t="s">
         <v>231</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="32" t="s">
-        <v>233</v>
-      </c>
       <c r="B3" s="32" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>242</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="33"/>
       <c r="B4" s="33"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="C5" s="34">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="34">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="34" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C9" s="34">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="C10" s="34">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="B8" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="B9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="B10" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
-        <v>236</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="34" t="s">
         <v>174</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3418,10 +3430,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.125" customWidth="1"/>
     <col min="2" max="2" width="12.375" customWidth="1"/>
@@ -3429,7 +3441,7 @@
     <col min="4" max="4" width="11.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -3446,7 +3458,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3457,7 +3469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -3471,7 +3483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3488,9 +3500,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3516,12 +3528,12 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>139</v>
       </c>
@@ -3538,7 +3550,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>138</v>
       </c>
@@ -3549,7 +3561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>141</v>
       </c>
@@ -3563,7 +3575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>173</v>
       </c>
@@ -3580,9 +3592,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C5">
         <v>1</v>

</xml_diff>

<commit_message>
feat(KeyedList): support enum as key type
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF067D70-BD8E-4417-AC8F-C6B115A2E5AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3528500-B395-4650-BB2F-60551B36D2FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="5070" windowWidth="24840" windowHeight="13740" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="6210" yWindow="2565" windowWidth="31050" windowHeight="17070" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="248">
   <si>
     <t>2020-01-01  05:00:00</t>
   </si>
@@ -740,10 +740,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>ServerConfName</t>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>进程名</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
@@ -757,27 +753,9 @@
     <t>gamesvr</t>
   </si>
   <si>
-    <t>HeadFrameConf</t>
-  </si>
-  <si>
     <t>activitysvr</t>
   </si>
   <si>
-    <t>ActivityConf</t>
-  </si>
-  <si>
-    <t>ChapterConf</t>
-  </si>
-  <si>
-    <t>CollectionConf</t>
-  </si>
-  <si>
-    <t>ExchangeConf</t>
-  </si>
-  <si>
-    <t>SectionConf</t>
-  </si>
-  <si>
     <t>配置Sheet名</t>
   </si>
   <si>
@@ -793,13 +771,28 @@
     <t>条件值</t>
   </si>
   <si>
-    <t>[Conf]&lt;string&gt;</t>
-  </si>
-  <si>
     <t>map&lt;string, Server&gt;</t>
   </si>
   <si>
     <t>[Condition]int32</t>
+  </si>
+  <si>
+    <t>CONF_TYPE_CLOUD</t>
+  </si>
+  <si>
+    <t>CONF_TYPE_REMOTE</t>
+  </si>
+  <si>
+    <t>CONF_TYPE_LOCAL</t>
+  </si>
+  <si>
+    <t>CONF_TYPE_UNKNOWN</t>
+  </si>
+  <si>
+    <t>ServerConfType</t>
+  </si>
+  <si>
+    <t>[Conf]&lt;enum&lt;.ConfType&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -3285,13 +3278,13 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.25" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="25.875" style="34" customWidth="1"/>
     <col min="3" max="3" width="28.375" style="34" customWidth="1"/>
     <col min="4" max="4" width="22.25" customWidth="1"/>
   </cols>
@@ -3301,24 +3294,24 @@
         <v>229</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D1" s="32" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B2" s="32" t="s">
         <v>247</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>53</v>
@@ -3326,16 +3319,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="D3" s="32" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3346,10 +3339,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C5" s="34">
         <v>1</v>
@@ -3368,20 +3361,20 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="34" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C9" s="34">
         <v>9</v>
@@ -3392,7 +3385,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C10" s="34">
         <v>9</v>
@@ -3403,20 +3396,20 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="34" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>174</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -3502,7 +3495,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -3594,7 +3587,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C5">
         <v>1</v>

</xml_diff>

<commit_message>
fix(KeyedList): avoid unpopulated(scaler type's default value) field, auto populate legal nested message field
</commit_message>
<xml_diff>
--- a/test/testdata/Test.xlsx
+++ b/test/testdata/Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\tableau\test\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3528500-B395-4650-BB2F-60551B36D2FF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7EBDBC-5E3E-4F5F-9A13-4D9C34763427}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6210" yWindow="2565" windowWidth="31050" windowHeight="17070" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
+    <workbookView xWindow="-4125" yWindow="6735" windowWidth="31050" windowHeight="17070" activeTab="4" xr2:uid="{789FF568-E43D-DA4B-9C6E-0C49405D287E}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="2" r:id="rId1"/>
@@ -774,9 +774,6 @@
     <t>map&lt;string, Server&gt;</t>
   </si>
   <si>
-    <t>[Condition]int32</t>
-  </si>
-  <si>
     <t>CONF_TYPE_CLOUD</t>
   </si>
   <si>
@@ -793,6 +790,9 @@
   </si>
   <si>
     <t>[Conf]&lt;enum&lt;.ConfType&gt;&gt;</t>
+  </si>
+  <si>
+    <t>[Condition]&lt;int32&gt;</t>
   </si>
 </sst>
 </file>
@@ -3278,7 +3278,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3294,7 +3294,7 @@
         <v>229</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>236</v>
@@ -3308,10 +3308,10 @@
         <v>240</v>
       </c>
       <c r="B2" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>247</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>241</v>
       </c>
       <c r="D2" s="32" t="s">
         <v>53</v>
@@ -3342,10 +3342,10 @@
         <v>233</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C5" s="34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5">
         <v>113</v>
@@ -3353,10 +3353,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" s="34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>114</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3364,17 +3364,17 @@
         <v>234</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="34">
         <v>9</v>
@@ -3385,7 +3385,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" s="34">
         <v>9</v>
@@ -3396,12 +3396,12 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="34" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>232</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>